<commit_message>
update on 25 Apr 2023
</commit_message>
<xml_diff>
--- a/region-cooking.xlsx
+++ b/region-cooking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bikash/TEA-cook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00-Bikash\01-cooking\01-analysis-files\TEA-cook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74B54E8-DDC0-BC4D-9AEC-49E2AC99CFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B2525B-620D-4B3F-B618-3972E09F87DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{A1E78D55-17B1-CA4C-9F0B-557606749D1E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1E78D55-17B1-CA4C-9F0B-557606749D1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -221,7 +221,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{78B7DE9B-2AD7-47A9-A510-B256A9DA176D}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -234,7 +236,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -522,7 +524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -532,20 +534,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C90523-4C47-1D43-A85C-B69174CF71A1}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="6"/>
-    <col min="2" max="2" width="73.1640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="74.83203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="47.1640625" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" style="6"/>
+    <col min="2" max="2" width="73.19921875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="74.796875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="47.19921875" customWidth="1"/>
     <col min="7" max="7" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -565,7 +567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -585,7 +587,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -605,7 +607,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -625,7 +627,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -636,7 +638,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -647,7 +649,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>

</xml_diff>